<commit_message>
mostly done with the excel, there are no more errors from the script only need to change hardpoints in excel
</commit_message>
<xml_diff>
--- a/sm_car_ARTTU_Brakes.xlsx
+++ b/sm_car_ARTTU_Brakes.xlsx
@@ -1,27 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Desktop/FSAE/Motor Control/VehicleModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrei/Desktop/FSAE/Vehicle Model/Main/Develop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9900EF73-C9D3-9041-8691-53988BB0A893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0904922E-0CC0-4A49-BD78-FD3AFE72E130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="2060" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16820" yWindow="2460" windowWidth="15960" windowHeight="18080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Front" sheetId="1" r:id="rId1"/>
-    <sheet name="Rear" sheetId="2" r:id="rId2"/>
+    <sheet name="Brakes" sheetId="3" r:id="rId1"/>
+    <sheet name="Axle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Axle2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
   <si>
     <t>Category</t>
   </si>
@@ -38,52 +55,40 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Asdas</t>
-  </si>
-  <si>
     <t>Instance</t>
   </si>
   <si>
-    <t>Aaaadd</t>
-  </si>
-  <si>
     <t>class</t>
   </si>
   <si>
-    <t>Dddd</t>
-  </si>
-  <si>
     <t>DiscAndPad</t>
   </si>
   <si>
-    <t>meanRadius</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>MuStatic</t>
+    <t>rMuStatic</t>
   </si>
   <si>
     <t>(0-1)</t>
   </si>
   <si>
-    <t>MuKinetic</t>
-  </si>
-  <si>
-    <t>Transition</t>
+    <t>rMuKinetic</t>
+  </si>
+  <si>
+    <t>nTransition</t>
   </si>
   <si>
     <t>rad/s</t>
   </si>
   <si>
-    <t>Viscous</t>
+    <t>dViscous</t>
   </si>
   <si>
     <t>N*m/(rad/s)</t>
   </si>
   <si>
-    <t>Pads</t>
+    <t>NPads</t>
   </si>
   <si>
     <t>Number of pads</t>
@@ -92,25 +97,40 @@
     <t>Caliper</t>
   </si>
   <si>
-    <t>CylinderDiameter</t>
+    <t>lCylinderDiameter</t>
   </si>
   <si>
     <t>pMax</t>
   </si>
   <si>
-    <t>fActuatorCutof</t>
+    <t>Bar</t>
   </si>
   <si>
     <t>1/sec</t>
   </si>
   <si>
-    <t>Front</t>
+    <t>Axle1</t>
+  </si>
+  <si>
+    <t>Axle2</t>
   </si>
   <si>
     <t>SHEET</t>
   </si>
   <si>
-    <t>[10 12 3]</t>
+    <t>PedalAbstract_DiscDisc</t>
+  </si>
+  <si>
+    <t>Axle2_PedalAbstract_DiscDisc_FSAE_Achilles</t>
+  </si>
+  <si>
+    <t>Brakes</t>
+  </si>
+  <si>
+    <t>lMeanRadius</t>
+  </si>
+  <si>
+    <t>fActuatorCutoff</t>
   </si>
 </sst>
 </file>
@@ -372,7 +392,7 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -384,7 +404,7 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -399,7 +419,7 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -411,8 +431,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1544,11 +1564,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7260810A-C070-C644-A900-448663B64E86}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1556,7 +1671,7 @@
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.83203125" style="1"/>
@@ -1582,150 +1697,146 @@
         <v>4</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="8"/>
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="12" t="s">
         <v>29</v>
       </c>
+      <c r="C5" s="12">
+        <v>0.107</v>
+      </c>
       <c r="D5" s="13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="16">
-        <v>1</v>
+        <v>0.35</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="16">
-        <v>22</v>
+        <v>0.35</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" s="16">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" s="16">
-        <v>5</v>
+        <v>1E-3</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" s="12">
-        <v>3</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="16">
-        <v>3</v>
-      </c>
-      <c r="D12" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C13" s="21">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E13" s="24"/>
     </row>
@@ -1742,18 +1853,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.83203125" style="1"/>
@@ -1779,150 +1892,146 @@
         <v>4</v>
       </c>
       <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2" s="8"/>
       <c r="D2" s="9"/>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C5" s="12">
-        <v>121</v>
+        <v>0.107</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="19"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="15" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="16">
-        <v>22</v>
+        <v>0.35</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8" s="16">
-        <v>4</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9" s="16">
-        <v>5</v>
+        <v>1E-3</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" s="21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" s="12">
-        <v>3</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27"/>
       <c r="B12" s="15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="16">
-        <v>3</v>
-      </c>
-      <c r="D12" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="27"/>
       <c r="B13" s="20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C13" s="21">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E13" s="24"/>
     </row>
@@ -1937,4 +2046,329 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9557458c-24b5-4c97-84ed-4c402655f54f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72e3c584-9879-4b35-b9d8-6a248c93e240" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009342B7EAA7728A4FA80A5CCAFE8D7EAF" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d037a5681ee6af0e7b5b5d0a2f99b20">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9557458c-24b5-4c97-84ed-4c402655f54f" xmlns:ns3="72e3c584-9879-4b35-b9d8-6a248c93e240" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="966978c8b125399653e7c255ac8e342d" ns2:_="" ns3:_="">
+    <xsd:import namespace="9557458c-24b5-4c97-84ed-4c402655f54f"/>
+    <xsd:import namespace="72e3c584-9879-4b35-b9d8-6a248c93e240"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9557458c-24b5-4c97-84ed-4c402655f54f" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="15" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="16" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a4a520e9-238f-4391-a566-21dd42474770" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="26" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="72e3c584-9879-4b35-b9d8-6a248c93e240" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="18" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="19" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{0d80220e-f9c1-4e35-9963-4ab067410620}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="72e3c584-9879-4b35-b9d8-6a248c93e240">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B5EDD56-952D-478D-9D58-1BE1EB9705F0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDA86A2E-D661-48BC-9909-67BBA76E0E88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9557458c-24b5-4c97-84ed-4c402655f54f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="72e3c584-9879-4b35-b9d8-6a248c93e240"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF7FF854-0D1C-4898-962F-3D7B24E6D626}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9557458c-24b5-4c97-84ed-4c402655f54f"/>
+    <ds:schemaRef ds:uri="72e3c584-9879-4b35-b9d8-6a248c93e240"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>